<commit_message>
Ordner Pyworld3_Update zum publishen vorbereitet
</commit_message>
<xml_diff>
--- a/Durchläufe/Größere Grid resolution/60/Nachbearbeitung_23_03_04_17_10.xlsx
+++ b/Durchläufe/Größere Grid resolution/60/Nachbearbeitung_23_03_04_17_10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim Schell\Documents\GitHub\Limits-to-Growth-Masterprojekt-TH-Koeln-2022\Durchläufe\Größere Grid resolution\60\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA04DBCE-8C25-41BD-9462-96A7380FDDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDC99A7-B6A5-4DC6-BC5E-78B0E8DF17C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1438,7 +1438,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" baseline="0"/>
-              <a:t> Change</a:t>
+              <a:t> Change, hohe Resolution</a:t>
             </a:r>
             <a:endParaRPr lang="de-DE"/>
           </a:p>
@@ -1574,19 +1574,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>2.4845000000000006E-2</c:v>
+                  <c:v>-2.4845000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.78817729999999986</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5427999999999933E-2</c:v>
+                  <c:v>-2.5427999999999933E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.13204399999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.9210399999999949E-2</c:v>
+                  <c:v>-9.9210399999999949E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.5186666666666699E-2</c:v>
@@ -1595,13 +1595,13 @@
                   <c:v>0.99832999999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.1150000000000049E-2</c:v>
+                  <c:v>-1.1150000000000049E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.1638499999999996E-2</c:v>
+                  <c:v>-1.1638499999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.50118571428571435</c:v>
+                  <c:v>-0.50118571428571435</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.43674485099999993</c:v>
@@ -1613,13 +1613,13 @@
                   <c:v>3.1100504999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.11476</c:v>
+                  <c:v>-0.11476</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.4299799999999999E-2</c:v>
+                  <c:v>-7.4299799999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.97909999999999997</c:v>
+                  <c:v>-0.97909999999999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0.65499999999999992</c:v>
@@ -1634,10 +1634,10 @@
                   <c:v>0.49038500000000007</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.2645791439241579E-2</c:v>
+                  <c:v>-9.2645791439241579E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.4503000000000044E-2</c:v>
+                  <c:v>-1.4503000000000044E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7837,8 +7837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B18376-9D15-4F7B-9DDA-34955610ECF9}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C36"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8275,8 +8275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86BCBB9C-0525-46F8-B6AB-26471E85C070}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B1:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8573,8 +8573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED61EA00-2246-4314-8737-2A6D310466A4}">
   <dimension ref="B1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8627,8 +8627,8 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <f>ABS(D2-E2)/E2</f>
-        <v>2.4845000000000006E-2</v>
+        <f>(D2-E2)/E2</f>
+        <v>-2.4845000000000006E-2</v>
       </c>
       <c r="H2" t="s">
         <v>34</v>
@@ -8652,7 +8652,7 @@
         <v>20</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F23" si="0">ABS(D3-E3)/E3</f>
+        <f t="shared" ref="F3:F23" si="0">(D3-E3)/E3</f>
         <v>0.78817729999999986</v>
       </c>
       <c r="H3" t="s">
@@ -8678,7 +8678,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>2.5427999999999933E-2</v>
+        <v>-2.5427999999999933E-2</v>
       </c>
       <c r="H4" t="s">
         <v>32</v>
@@ -8728,7 +8728,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>9.9210399999999949E-2</v>
+        <v>-9.9210399999999949E-2</v>
       </c>
       <c r="H6" t="s">
         <v>39</v>
@@ -8803,7 +8803,7 @@
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>1.1150000000000049E-2</v>
+        <v>-1.1150000000000049E-2</v>
       </c>
       <c r="H9" t="s">
         <v>8</v>
@@ -8828,7 +8828,7 @@
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>1.1638499999999996E-2</v>
+        <v>-1.1638499999999996E-2</v>
       </c>
       <c r="H10" t="s">
         <v>35</v>
@@ -8853,7 +8853,7 @@
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>0.50118571428571435</v>
+        <v>-0.50118571428571435</v>
       </c>
       <c r="H11" t="s">
         <v>36</v>
@@ -8953,7 +8953,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>0.11476</v>
+        <v>-0.11476</v>
       </c>
       <c r="I15" s="5"/>
     </row>
@@ -8973,7 +8973,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>7.4299799999999999E-2</v>
+        <v>-7.4299799999999999E-2</v>
       </c>
       <c r="I16" s="2"/>
     </row>
@@ -8993,7 +8993,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>0.97909999999999997</v>
+        <v>-0.97909999999999997</v>
       </c>
       <c r="I17" s="2"/>
     </row>
@@ -9091,7 +9091,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>9.2645791439241579E-2</v>
+        <v>-9.2645791439241579E-2</v>
       </c>
       <c r="G22" s="2"/>
     </row>
@@ -9111,7 +9111,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>1.4503000000000044E-2</v>
+        <v>-1.4503000000000044E-2</v>
       </c>
       <c r="G23" s="2"/>
     </row>

</xml_diff>